<commit_message>
modifico archivosdiarios.php para que vaya a buscar la extension de los archivos BIND con la extension A,B,C para Octubre, Noviembre y Diciembre
</commit_message>
<xml_diff>
--- a/input/reporte_transacciones_21-10-2025_15-08-42.xlsx
+++ b/input/reporte_transacciones_21-10-2025_15-08-42.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="94">
   <si>
     <t>País</t>
   </si>
@@ -162,7 +162,7 @@
     <t>morellinicolas7@gmail.com</t>
   </si>
   <si>
-    <t>C11672</t>
+    <t>C11581</t>
   </si>
   <si>
     <t>CUIT</t>
@@ -177,7 +177,7 @@
     <t/>
   </si>
   <si>
-    <t>2025-10-15T15:12:07-03:00</t>
+    <t>2025-10-18T15:12:07-03:00</t>
   </si>
   <si>
     <t>APPROVED</t>
@@ -219,7 +219,7 @@
     <t>ARS</t>
   </si>
   <si>
-    <t>2025-10-15T15:13:07-03:00</t>
+    <t>2025-10-18T15:13:07-03:00</t>
   </si>
   <si>
     <t>CREDIT</t>
@@ -237,19 +237,19 @@
     <t>2025-10-10</t>
   </si>
   <si>
-    <t>2025-10-15T15:13:51-03:00</t>
+    <t>2025-10-18T15:13:51-03:00</t>
   </si>
   <si>
     <t>PREPAID</t>
   </si>
   <si>
-    <t>2025-10-15T15:15:17-03:00</t>
+    <t>2025-10-18T15:15:17-03:00</t>
   </si>
   <si>
     <t>QR</t>
   </si>
   <si>
-    <t>2025-10-15T15:15:58-03:00</t>
+    <t>2025-10-18T15:15:58-03:00</t>
   </si>
   <si>
     <t>AMEX</t>
@@ -261,7 +261,7 @@
     <t>MX</t>
   </si>
   <si>
-    <t>2025-10-15T17:11:31-03:00</t>
+    <t>2025-10-18T17:11:31-03:00</t>
   </si>
   <si>
     <t>CUOTA_SIMPLE</t>
@@ -270,10 +270,7 @@
     <t>USD</t>
   </si>
   <si>
-    <t>762471688</t>
-  </si>
-  <si>
-    <t>2025-10-15T17:12:23-03:00</t>
+    <t>2025-10-18T17:12:23-03:00</t>
   </si>
   <si>
     <t>REJECTED</t>
@@ -282,16 +279,10 @@
     <t>XXXXXXXXXXXX4129</t>
   </si>
   <si>
-    <t>192861357</t>
-  </si>
-  <si>
-    <t>2025-10-15T17:14:20-03:00</t>
-  </si>
-  <si>
-    <t>799676995</t>
-  </si>
-  <si>
-    <t>2025-10-15T17:32:08-03:00</t>
+    <t>2025-10-18T17:14:20-03:00</t>
+  </si>
+  <si>
+    <t>2025-10-18T17:32:08-03:00</t>
   </si>
   <si>
     <t>2025-10-15</t>
@@ -300,19 +291,10 @@
     <t>2025-10-27</t>
   </si>
   <si>
-    <t>173946229</t>
-  </si>
-  <si>
-    <t>2025-10-15T17:32:45-03:00</t>
+    <t>2025-10-18T17:32:45-03:00</t>
   </si>
   <si>
     <t>6</t>
-  </si>
-  <si>
-    <t>2025-10-17T17:14:20-03:00</t>
-  </si>
-  <si>
-    <t>2025-10-17T17:32:08-03:00</t>
   </si>
   <si>
     <t>2025-10-02T17:32:45-03:00</t>
@@ -807,7 +789,8 @@
         <v>51</v>
       </c>
       <c r="I2" s="2">
-        <v>3.7226979E7</v>
+        <f t="shared" ref="I2:I14" si="1">RANDBETWEEN(11111111,99999999)</f>
+        <v>45485020</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>52</v>
@@ -950,7 +933,8 @@
         <v>51</v>
       </c>
       <c r="I3" s="2">
-        <v>9.5292778E8</v>
+        <f t="shared" si="1"/>
+        <v>45473376</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>52</v>
@@ -1093,7 +1077,8 @@
         <v>51</v>
       </c>
       <c r="I4" s="2">
-        <v>6.22917541E8</v>
+        <f t="shared" si="1"/>
+        <v>77382117</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>52</v>
@@ -1236,7 +1221,8 @@
         <v>51</v>
       </c>
       <c r="I5" s="2">
-        <v>5.15349428E8</v>
+        <f t="shared" si="1"/>
+        <v>88391157</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>52</v>
@@ -1379,7 +1365,8 @@
         <v>51</v>
       </c>
       <c r="I6" s="2">
-        <v>6.5682584E7</v>
+        <f t="shared" si="1"/>
+        <v>27403502</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>52</v>
@@ -1522,7 +1509,8 @@
         <v>51</v>
       </c>
       <c r="I7" s="2">
-        <v>4.72632867E8</v>
+        <f t="shared" si="1"/>
+        <v>52268408</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>52</v>
@@ -1664,17 +1652,18 @@
       <c r="H8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>28630521</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="M8" s="2">
         <v>40008.54</v>
@@ -1695,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T8" s="2">
         <v>1.0</v>
@@ -1807,17 +1796,18 @@
       <c r="H9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>88</v>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>40585188</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M9" s="5">
         <v>150.02</v>
@@ -1838,7 +1828,7 @@
         <v>52</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>70</v>
@@ -1950,17 +1940,18 @@
       <c r="H10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>90</v>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>79217294</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M10" s="6">
         <v>16846.35</v>
@@ -2008,7 +1999,7 @@
         <v>90.83</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AC10" s="3" t="s">
         <v>61</v>
@@ -2041,7 +2032,7 @@
         <v>81.81</v>
       </c>
       <c r="AM10" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AN10" s="3" t="s">
         <v>64</v>
@@ -2093,17 +2084,18 @@
       <c r="H11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>94</v>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>88019694</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M11" s="6">
         <v>1111235.55</v>
@@ -2127,7 +2119,7 @@
         <v>69</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>59</v>
@@ -2151,7 +2143,7 @@
         <v>82.81</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AC11" s="3" t="s">
         <v>61</v>
@@ -2184,7 +2176,7 @@
         <v>74.07</v>
       </c>
       <c r="AM11" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AN11" s="3" t="s">
         <v>64</v>
@@ -2236,17 +2228,18 @@
       <c r="H12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>88</v>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>47823236</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M12" s="1">
         <v>150.02</v>
@@ -2267,7 +2260,7 @@
         <v>52</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>70</v>
@@ -2379,17 +2372,18 @@
       <c r="H13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>90</v>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>48389938</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M13" s="2">
         <v>115.25</v>
@@ -2437,7 +2431,7 @@
         <v>90.83</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>61</v>
@@ -2470,7 +2464,7 @@
         <v>81.81</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AN13" s="1" t="s">
         <v>64</v>
@@ -2522,17 +2516,18 @@
       <c r="H14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>94</v>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>47022645</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M14" s="2">
         <v>130.48</v>
@@ -2556,7 +2551,7 @@
         <v>69</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>59</v>
@@ -2580,7 +2575,7 @@
         <v>82.81</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>61</v>
@@ -2613,7 +2608,7 @@
         <v>74.07</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AN14" s="1" t="s">
         <v>64</v>

</xml_diff>